<commit_message>
Texturing done, working on camera rotation using mouse
</commit_message>
<xml_diff>
--- a/Project4/Dev IV Project Rubric.xlsx
+++ b/Project4/Dev IV Project Rubric.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -41,7 +41,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="A66" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -366,12 +366,15 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -929,11 +932,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,11 +1051,15 @@
       <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G30" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84))</f>
@@ -1060,11 +1067,11 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1072,7 +1079,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1201,11 +1208,11 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1410,11 +1417,15 @@
       <c r="D17" s="5">
         <v>2</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
+      <c r="E17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G17" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -2375,11 +2386,15 @@
       <c r="D60" s="5">
         <v>1</v>
       </c>
-      <c r="E60" s="2"/>
-      <c r="F60" s="3"/>
+      <c r="E60" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G60" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
@@ -2400,11 +2415,15 @@
       <c r="D61" s="5">
         <v>1</v>
       </c>
-      <c r="E61" s="2"/>
-      <c r="F61" s="3"/>
+      <c r="E61" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G61" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
@@ -2862,8 +2881,12 @@
       <c r="C83" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
+      <c r="D83" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
@@ -2882,8 +2905,12 @@
       <c r="C84" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
+      <c r="D84" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
@@ -3016,7 +3043,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3055,18 +3082,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with capital X!" sqref="C83:E84 F4:F81" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with capital X!" sqref="C83:E84 F4:F81">
       <formula1>IF(EXACT(C4,"X"),TRUE,FALSE)</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D80:D81 D3:D78 B3:C81" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D80:D81 D3:D78 B3:C81">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D79" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D79">
       <formula1>1</formula1>
       <formula2>6</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with roman numerals I, II, or III!" sqref="E4:E81" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with roman numerals I, II, or III!" sqref="E4:E81">
       <formula1>IF(EXACT(E4,"I"),TRUE,IF(EXACT(E4,"II"),TRUE,IF(EXACT(E4,"III"),TRUE,FALSE)))</formula1>
     </dataValidation>
   </dataValidations>
@@ -3082,7 +3109,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3099,7 +3126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Loading semi-works, can load simple obj file
</commit_message>
<xml_diff>
--- a/Project4/Dev IV Project Rubric.xlsx
+++ b/Project4/Dev IV Project Rubric.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -41,7 +41,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0">
+    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -368,13 +368,13 @@
     <t>X</t>
   </si>
   <si>
-    <t>III</t>
+    <t>I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -932,11 +932,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,19 +1059,19 @@
       </c>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G30" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84))</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1204,15 +1204,15 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="G17" s="16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -2881,12 +2881,8 @@
       <c r="C83" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>93</v>
-      </c>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
@@ -2905,12 +2901,8 @@
       <c r="C84" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>93</v>
-      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
@@ -3043,7 +3035,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3082,18 +3074,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with capital X!" sqref="C83:E84 F4:F81">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with capital X!" sqref="C83:E84 F4:F81" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>IF(EXACT(C4,"X"),TRUE,FALSE)</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D80:D81 D3:D78 B3:C81">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D80:D81 D3:D78 B3:C81" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D79">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D79" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>1</formula1>
       <formula2>6</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with roman numerals I, II, or III!" sqref="E4:E81">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with roman numerals I, II, or III!" sqref="E4:E81" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>IF(EXACT(E4,"I"),TRUE,IF(EXACT(E4,"II"),TRUE,IF(EXACT(E4,"III"),TRUE,FALSE)))</formula1>
     </dataValidation>
   </dataValidations>
@@ -3109,7 +3101,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3126,7 +3118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
All lights implemented, no movement on them however
</commit_message>
<xml_diff>
--- a/Project4/Dev IV Project Rubric.xlsx
+++ b/Project4/Dev IV Project Rubric.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -935,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1066,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84))</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84))</f>
@@ -1079,7 +1082,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1095,11 +1098,15 @@
       <c r="D5" s="5">
         <v>2</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>27</v>
@@ -1204,7 +1211,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
@@ -2444,7 +2451,9 @@
       <c r="D62" s="5">
         <v>1</v>
       </c>
-      <c r="E62" s="2"/>
+      <c r="E62" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F62" s="3"/>
       <c r="G62" s="16">
         <f t="shared" si="1"/>
@@ -2494,7 +2503,9 @@
       <c r="D64" s="5">
         <v>1</v>
       </c>
-      <c r="E64" s="2"/>
+      <c r="E64" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F64" s="3"/>
       <c r="G64" s="16">
         <f t="shared" si="1"/>
@@ -3035,7 +3046,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Rubric change and tweaks
</commit_message>
<xml_diff>
--- a/Project4/Dev IV Project Rubric.xlsx
+++ b/Project4/Dev IV Project Rubric.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="97">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -938,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,11 +1073,11 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1082,7 +1085,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1135,7 +1138,9 @@
       <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
@@ -1215,11 +1220,11 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1503,7 +1508,9 @@
       <c r="D20" s="5">
         <v>3</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="16">
         <f t="shared" si="0"/>
@@ -1606,11 +1613,15 @@
       <c r="D25" s="5">
         <v>2</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="3"/>
+      <c r="E25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G25" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -1631,11 +1642,15 @@
       <c r="D26" s="5">
         <v>2</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
+      <c r="E26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G26" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -1656,11 +1671,15 @@
       <c r="D27" s="5">
         <v>2</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="3"/>
+      <c r="E27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G27" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -1681,11 +1700,15 @@
       <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="3"/>
+      <c r="E28" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G28" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -1706,7 +1729,9 @@
       <c r="D29" s="5">
         <v>1</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="16">
         <f t="shared" si="0"/>
@@ -1731,7 +1756,9 @@
       <c r="D30" s="5">
         <v>1</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="16">
         <f t="shared" si="0"/>
@@ -1756,7 +1783,9 @@
       <c r="D31" s="5">
         <v>1</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="16">
         <f t="shared" ref="G31:G65" si="1" xml:space="preserve"> IF(EXACT(F31,"X"),IF(EXACT(E31,"I"),$B31,IF(EXACT(E31,"II"),$C31,IF(EXACT(E31,"III"),$D31,0))),0)</f>
@@ -1856,11 +1885,15 @@
       <c r="D35" s="5">
         <v>2</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="3"/>
+      <c r="E35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -1934,11 +1967,15 @@
       <c r="D39" s="5">
         <v>1</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="3"/>
+      <c r="E39" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G39" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -2240,11 +2277,15 @@
       <c r="D53" s="5">
         <v>2</v>
       </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="3"/>
+      <c r="E53" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G53" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
@@ -2265,7 +2306,9 @@
       <c r="D54" s="5">
         <v>2</v>
       </c>
-      <c r="E54" s="2"/>
+      <c r="E54" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="F54" s="3"/>
       <c r="G54" s="16">
         <f t="shared" si="1"/>
@@ -2454,10 +2497,12 @@
       <c r="E62" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F62" s="3"/>
+      <c r="F62" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G62" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
@@ -2506,10 +2551,12 @@
       <c r="E64" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F64" s="3"/>
+      <c r="F64" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G64" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
@@ -2707,7 +2754,9 @@
       <c r="D74" s="5">
         <v>3</v>
       </c>
-      <c r="E74" s="2"/>
+      <c r="E74" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="F74" s="3"/>
       <c r="G74" s="16">
         <f t="shared" si="4"/>
@@ -2892,8 +2941,12 @@
       <c r="C83" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
+      <c r="D83" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
@@ -2912,8 +2965,12 @@
       <c r="C84" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
+      <c r="D84" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>

</xml_diff>

<commit_message>
removed stuff, skybox done, resize correctly done, working on instancing
</commit_message>
<xml_diff>
--- a/Project4/Dev IV Project Rubric.xlsx
+++ b/Project4/Dev IV Project Rubric.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -41,7 +41,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="A66" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="97">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -380,7 +380,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -938,11 +938,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1224,7 +1224,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1511,10 +1511,12 @@
       <c r="E20" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G20" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -2309,10 +2311,12 @@
       <c r="E54" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F54" s="3"/>
+      <c r="F54" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G54" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
@@ -3103,7 +3107,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3142,18 +3146,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with capital X!" sqref="C83:E84 F4:F81" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with capital X!" sqref="C83:E84 F4:F81">
       <formula1>IF(EXACT(C4,"X"),TRUE,FALSE)</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D80:D81 D3:D78 B3:C81" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D80:D81 D3:D78 B3:C81">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D79" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D79">
       <formula1>1</formula1>
       <formula2>6</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with roman numerals I, II, or III!" sqref="E4:E81" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with roman numerals I, II, or III!" sqref="E4:E81">
       <formula1>IF(EXACT(E4,"I"),TRUE,IF(EXACT(E4,"II"),TRUE,IF(EXACT(E4,"III"),TRUE,FALSE)))</formula1>
     </dataValidation>
   </dataValidations>
@@ -3169,7 +3173,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3186,7 +3190,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Finished up project, yay
</commit_message>
<xml_diff>
--- a/Project4/Dev IV Project Rubric.xlsx
+++ b/Project4/Dev IV Project Rubric.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -41,7 +41,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0">
+    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -380,7 +380,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -938,11 +938,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,15 +1077,15 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1141,10 +1141,12 @@
       <c r="E6" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84)  &gt; 18, SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84) - 18,0)</f>
@@ -1156,7 +1158,7 @@
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) - 18,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="15">
@@ -1216,7 +1218,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
@@ -1224,7 +1226,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1734,10 +1736,12 @@
       <c r="E29" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F29" s="3"/>
+      <c r="F29" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G29" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -1761,10 +1765,12 @@
       <c r="E30" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G30" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1788,10 +1794,12 @@
       <c r="E31" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G31" s="16">
         <f t="shared" ref="G31:G65" si="1" xml:space="preserve"> IF(EXACT(F31,"X"),IF(EXACT(E31,"I"),$B31,IF(EXACT(E31,"II"),$C31,IF(EXACT(E31,"III"),$D31,0))),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -2761,10 +2769,12 @@
       <c r="E74" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F74" s="3"/>
+      <c r="F74" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G74" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
@@ -3146,18 +3156,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with capital X!" sqref="C83:E84 F4:F81">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with capital X!" sqref="C83:E84 F4:F81" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>IF(EXACT(C4,"X"),TRUE,FALSE)</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D80:D81 D3:D78 B3:C81">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D80:D81 D3:D78 B3:C81" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D79">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D79" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>1</formula1>
       <formula2>6</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with roman numerals I, II, or III!" sqref="E4:E81">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with roman numerals I, II, or III!" sqref="E4:E81" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>IF(EXACT(E4,"I"),TRUE,IF(EXACT(E4,"II"),TRUE,IF(EXACT(E4,"III"),TRUE,FALSE)))</formula1>
     </dataValidation>
   </dataValidations>
@@ -3173,7 +3183,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3190,7 +3200,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>